<commit_message>
added memory overhead to runtime_data
</commit_message>
<xml_diff>
--- a/runtime_data.xlsx
+++ b/runtime_data.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
   <si>
     <t>Variable assignment funct</t>
   </si>
@@ -39,6 +39,9 @@
   </si>
   <si>
     <t>Totient function</t>
+  </si>
+  <si>
+    <t>Array assignment</t>
   </si>
 </sst>
 </file>
@@ -1200,6 +1203,562 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>Performance With/Without Taint Tracking: Memory Used</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>TT</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$15:$G$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>512.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1024.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2048.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4096.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8192.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$16:$G$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>9006.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10687.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11149.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12797.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17952.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>22269.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>No TT</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$15:$G$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>512.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1024.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2048.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4096.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8192.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$17:$G$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>8264.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8504.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10689.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11419.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12371.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12327.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2073771376"/>
+        <c:axId val="-2073637344"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2073771376"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>n</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2073637344"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2073637344"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>KB Bytes Allocated</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2073771376"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1280,6 +1839,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -1797,6 +2396,522 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2346,16 +3461,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>635000</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>393700</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2371,6 +3486,38 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>469900</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>139700</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2642,10 +3789,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2854,6 +4001,81 @@
       <c r="G12">
         <f t="shared" ref="G12" si="5">G10/G11</f>
         <v>2.2706729575366276</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B15">
+        <v>256</v>
+      </c>
+      <c r="C15">
+        <v>512</v>
+      </c>
+      <c r="D15">
+        <f>2^10</f>
+        <v>1024</v>
+      </c>
+      <c r="E15">
+        <f>2^11</f>
+        <v>2048</v>
+      </c>
+      <c r="F15">
+        <f>2^12</f>
+        <v>4096</v>
+      </c>
+      <c r="G15">
+        <f>2^13</f>
+        <v>8192</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <v>9006</v>
+      </c>
+      <c r="C16">
+        <v>10687</v>
+      </c>
+      <c r="D16">
+        <v>11149</v>
+      </c>
+      <c r="E16">
+        <v>12797</v>
+      </c>
+      <c r="F16">
+        <v>17952</v>
+      </c>
+      <c r="G16">
+        <v>22269</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17">
+        <v>8264</v>
+      </c>
+      <c r="C17">
+        <v>8504</v>
+      </c>
+      <c r="D17">
+        <v>10689</v>
+      </c>
+      <c r="E17">
+        <v>11419</v>
+      </c>
+      <c r="F17">
+        <v>12371</v>
+      </c>
+      <c r="G17">
+        <v>12327</v>
       </c>
     </row>
   </sheetData>

</xml_diff>